<commit_message>
add Label (Drug) api
</commit_message>
<xml_diff>
--- a/assets/data/label.xlsx
+++ b/assets/data/label.xlsx
@@ -21,21 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
-    <t>ชื่อยา</t>
-  </si>
-  <si>
-    <t>ข้อบ่งใช้</t>
-  </si>
-  <si>
-    <t>คำเตือนบนฉลากยา</t>
-  </si>
-  <si>
-    <t>ข้อความบนฉลากยาเสริม</t>
-  </si>
-  <si>
-    <t>หมายเหตุ</t>
-  </si>
-  <si>
     <t>Paracetamol tablet</t>
   </si>
   <si>
@@ -130,12 +115,6 @@
 - 500 มิลลิกรัม (8 เม็ด)
 - 325 มิลลิกรัม (12 เม็ด)
 </t>
-  </si>
-  <si>
-    <t>Amoxycillin(ชนิดเม็ด)</t>
-  </si>
-  <si>
-    <t>Amoxycillin(ชนิดน้ำ)</t>
   </si>
   <si>
     <t xml:space="preserve">1. ควรระวังในการกินร่วมกับยาที่มีพาราเซตามอลเป็นส่วนผสมอยู่ด้วย เช่น ยาแผงบรรเทาหวัด ยาแก้ปวดกล้ามเนื้อ เป็นต้น เพราะอาจทำให้ได้รับยาซ้ำซ้อนจนเกินขนาด
@@ -265,6 +244,27 @@
 3. ควรแจ้งให้แพทย์หรือเภสัชกรทราบ ถ้าท่านได้รับยาอื่นอยู่ โดยเฉพาะยาฆ่าเชื้อแบคทีเรีย (ชนิดอิริโทรมัยซิน คลาริโทรมัยซิน) ยาฆ่าเชื้อรา (ชนิดคีโตโคนาโซน และไอทราโคนาโซน)     ยากลุ่มสแตติน ยาควบคุมความดันเลือด (ชนิดดิลไทอะเซ็ม หรือเวอราปามิล) เพราะอาจเกิดปฏิกิริยาตีกันกับยานี้
 4. หากท่านเป็นโรคตับ โรคไต วางแผนตั้งครรภ์หรือกำลังตั้งครรภ์ หรือให้นมบุตร ควรแจ้งให้แพทย์หรือเภสัชกรทราบ
 </t>
+  </si>
+  <si>
+    <t>drug_name</t>
+  </si>
+  <si>
+    <t>term_of_use</t>
+  </si>
+  <si>
+    <t>warning_label</t>
+  </si>
+  <si>
+    <t>text_label</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>Amoxycillin (ชนิดน้ำ)</t>
+  </si>
+  <si>
+    <t>Amoxycillin (ชนิดเม็ด)</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+      <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -831,36 +831,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,16 +893,16 @@
     </row>
     <row r="7" spans="1:5" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -922,16 +922,16 @@
     </row>
     <row r="10" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7"/>
     </row>
@@ -958,16 +958,16 @@
     </row>
     <row r="14" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E14" s="7"/>
     </row>
@@ -987,16 +987,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E17" s="7"/>
     </row>
@@ -1016,16 +1016,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -1038,16 +1038,16 @@
     </row>
     <row r="22" spans="1:5" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -1074,16 +1074,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -1096,16 +1096,16 @@
     </row>
     <row r="28" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E28" s="7"/>
     </row>
@@ -1181,16 +1181,16 @@
     </row>
     <row r="39" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E39" s="7"/>
     </row>
@@ -1210,16 +1210,16 @@
     </row>
     <row r="42" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E42" s="7"/>
     </row>
@@ -1260,16 +1260,16 @@
     </row>
     <row r="48" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E48" s="7"/>
     </row>
@@ -1317,16 +1317,16 @@
     </row>
     <row r="55" spans="1:5" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E55" s="7"/>
     </row>
@@ -1367,16 +1367,16 @@
     </row>
     <row r="61" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="E61" s="7"/>
     </row>
@@ -1403,16 +1403,16 @@
     </row>
     <row r="65" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E65" s="7"/>
     </row>

</xml_diff>